<commit_message>
style: Atualiza design da aplicação e melhora layout
</commit_message>
<xml_diff>
--- a/teste2.xlsx
+++ b/teste2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Documents\ZTE-MASTER\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Documents\ONU-TERMINATOR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Serial</t>
   </si>
@@ -32,10 +32,22 @@
     <t>Name</t>
   </si>
   <si>
-    <t>ZTEGD1BBDFFC</t>
-  </si>
-  <si>
-    <t>eliasbertani</t>
+    <t>leidiomar_corsini.STM</t>
+  </si>
+  <si>
+    <t>ZTEGD1D29299</t>
+  </si>
+  <si>
+    <t>ZTEGD2B331A9</t>
+  </si>
+  <si>
+    <t>leaniroliveira</t>
+  </si>
+  <si>
+    <t>laboratoriolidersantaluzia</t>
+  </si>
+  <si>
+    <t>ZTEGD1E1FBFB</t>
   </si>
 </sst>
 </file>
@@ -353,16 +365,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -375,10 +387,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>